<commit_message>
tidied up documentation folder to have updated Documentation.xlsx
tidied up documentation folder to have updated Documentation.xlsx
</commit_message>
<xml_diff>
--- a/documents/Documentations.xlsx
+++ b/documents/Documentations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\project-g5t4\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Fake-repo-for-SPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C896592-14AF-4338-B65C-A7FE7F20FEC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEC70AF-2DC9-476E-849B-B6247B2E7097}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{DD198B49-0243-4A5C-9C43-27E058F9B647}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="21">
   <si>
     <t>Iteration</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>Leonard, See Hoe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leonard, See Hoe </t>
+  </si>
+  <si>
+    <t>Serene, See Hoe</t>
   </si>
 </sst>
 </file>
@@ -182,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -222,6 +228,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -643,7 +652,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -730,13 +739,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
@@ -750,13 +759,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -766,6 +775,18 @@
       <c r="K6" s="13"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="15">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>

</xml_diff>